<commit_message>
Corrected some values and errors
</commit_message>
<xml_diff>
--- a/Versuch10/datasets/schwing1.xlsx
+++ b/Versuch10/datasets/schwing1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michele Calvanese\Uni\Grundpraktikum\Versuch10\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C831339D-4ABC-4E1F-BEA9-CA7A8E135CD2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{825D1683-4873-4A84-914B-2F326E6F546A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17040" windowHeight="5916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -977,7 +977,7 @@
   <dimension ref="A1:AC12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1080,7 +1080,7 @@
         <v>3.2</v>
       </c>
       <c r="C2">
-        <v>0.2</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="F2">
         <f>C2/SQRT(D2)</f>
-        <v>0.11547005383792516</v>
+        <v>8.1406387955737236E-2</v>
       </c>
       <c r="G2">
         <f>2*PI()/E2</f>
@@ -1109,14 +1109,14 @@
         <v>1.0628446082305574</v>
       </c>
       <c r="K2">
-        <f>C2/SQRT(D2)</f>
-        <v>0.11547005383792516</v>
+        <f t="shared" ref="K2:K11" si="0">C2/SQRT(D2)</f>
+        <v>8.1406387955737236E-2</v>
       </c>
       <c r="L2">
         <v>8.83</v>
       </c>
       <c r="M2">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="N2">
         <v>16</v>
@@ -1138,36 +1138,36 @@
         <v>19.600000000000001</v>
       </c>
       <c r="T2">
-        <f t="shared" ref="T2:T11" si="0">4000*N2*9.8/(P2^2*PI())</f>
-        <v>779.85922115028723</v>
+        <f>4000*N2*9.806/(P2^2*PI())</f>
+        <v>780.33668597956284</v>
       </c>
       <c r="U2">
         <f>T2*SQRT((O2/N2)^2+4*(Q2/P2)^2)</f>
-        <v>26.247940201611573</v>
+        <v>26.264010369081944</v>
       </c>
       <c r="V2">
         <f>R2+T2</f>
-        <v>98779.859221150284</v>
+        <v>98780.336685979564</v>
       </c>
       <c r="W2">
         <f>SQRT(S2^2+U2^2)</f>
-        <v>32.758424333709598</v>
+        <v>32.771302089896338</v>
       </c>
       <c r="X2">
-        <f>10^6*64*L2*N2/(E2^2*P2^4*(R2+T2))</f>
-        <v>1.2275943460114138</v>
+        <f t="shared" ref="X2:X11" si="1">10^6*64*L2*N2/(E2^2*P2^4*(R2+T2))</f>
+        <v>1.2275884123089735</v>
       </c>
       <c r="Y2">
-        <f>X2*SQRT((O2/N2)^2+(M2/L2)^2+4*(K2/E2)^2+16*(Q2/P2)^2+(W2/V2^2))</f>
-        <v>0.27064160391557401</v>
+        <f t="shared" ref="Y2:Y11" si="2">X2*SQRT((O2/N2)^2+(M2/L2)^2+4*(K2/E2)^2+16*(Q2/P2)^2+(W2/V2^2))</f>
+        <v>0.19411235824513914</v>
       </c>
       <c r="Z2">
         <f>10^6*64*L2*N2/(J2^2*P2^4*(R2+T2))</f>
-        <v>1.2364392393213171</v>
+        <v>1.2364332628661832</v>
       </c>
       <c r="AB2">
         <f>AVERAGE(X2:X11)</f>
-        <v>1.2006629491547423</v>
+        <v>1.2006571456279542</v>
       </c>
       <c r="AC2">
         <v>0</v>
@@ -1181,21 +1181,22 @@
         <v>4.37</v>
       </c>
       <c r="C3">
-        <v>0.2</v>
+        <f>C2</f>
+        <v>0.14099999999999999</v>
       </c>
       <c r="D3">
         <v>4</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E11" si="1">B3/D3</f>
+        <f t="shared" ref="E3:E11" si="3">B3/D3</f>
         <v>1.0925</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F11" si="2">C3/SQRT(D3)</f>
-        <v>0.1</v>
+        <f t="shared" ref="F3:F11" si="4">C3/SQRT(D3)</f>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G11" si="3">2*PI()/E3</f>
+        <f t="shared" ref="G3:G11" si="5">2*PI()/E3</f>
         <v>5.7511993658394385</v>
       </c>
       <c r="H3">
@@ -1203,16 +1204,16 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I11" si="4">SQRT(G3^2+H3^2/4)</f>
+        <f t="shared" ref="I3:I11" si="6">SQRT(G3^2+H3^2/4)</f>
         <v>5.7728930481719445</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J11" si="5">2*PI()/I3</f>
+        <f t="shared" ref="J3:J11" si="7">2*PI()/I3</f>
         <v>1.0883945458108273</v>
       </c>
       <c r="K3">
-        <f>C3/SQRT(D3)</f>
-        <v>0.1</v>
+        <f t="shared" si="0"/>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="L3">
         <f>L2</f>
@@ -1220,13 +1221,14 @@
       </c>
       <c r="M3">
         <f>M2</f>
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="N3">
         <f>N2</f>
         <v>16</v>
       </c>
       <c r="O3">
+        <f>O2</f>
         <v>0.5</v>
       </c>
       <c r="P3">
@@ -1234,6 +1236,7 @@
         <v>16</v>
       </c>
       <c r="Q3">
+        <f>Q2</f>
         <v>0.1</v>
       </c>
       <c r="R3">
@@ -1241,36 +1244,36 @@
         <v>98000</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S11" si="6">R3*0.0002</f>
+        <f t="shared" ref="S3:S11" si="8">R3*0.0002</f>
         <v>19.600000000000001</v>
       </c>
       <c r="T3">
-        <f t="shared" si="0"/>
-        <v>779.85922115028723</v>
+        <f t="shared" ref="T3:T11" si="9">4000*N3*9.806/(P3^2*PI())</f>
+        <v>780.33668597956284</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U11" si="7">T3*SQRT((O3/N3)^2+4*(Q3/P3)^2)</f>
-        <v>26.247940201611573</v>
+        <f t="shared" ref="U3:U11" si="10">T3*SQRT((O3/N3)^2+4*(Q3/P3)^2)</f>
+        <v>26.264010369081944</v>
       </c>
       <c r="V3">
-        <f t="shared" ref="V3:V11" si="8">R3+T3</f>
-        <v>98779.859221150284</v>
+        <f t="shared" ref="V3:V11" si="11">R3+T3</f>
+        <v>98780.336685979564</v>
       </c>
       <c r="W3">
-        <f t="shared" ref="W3:W11" si="9">SQRT(S3^2+U3^2)</f>
-        <v>32.758424333709598</v>
+        <f t="shared" ref="W3:W11" si="12">SQRT(S3^2+U3^2)</f>
+        <v>32.771302089896338</v>
       </c>
       <c r="X3">
-        <f>10^6*64*L3*N3/(E3^2*P3^4*(R3+T3))</f>
-        <v>1.1702251712204017</v>
+        <f t="shared" si="1"/>
+        <v>1.1702195148177172</v>
       </c>
       <c r="Y3">
-        <f>X3*SQRT((O3/N3)^2+(M3/L3)^2+4*(K3/E3)^2+16*(Q3/P3)^2+(W3/V3^2))</f>
-        <v>0.21968812288076248</v>
+        <f t="shared" si="2"/>
+        <v>0.15857401832191509</v>
       </c>
       <c r="Z3">
-        <f t="shared" ref="Z3:Z11" si="10">10^6*64*L3*N3/(J3^2*P3^4*(R3+T3))</f>
-        <v>1.1790700645303058</v>
+        <f t="shared" ref="Z3:Z11" si="13">10^6*64*L3*N3/(J3^2*P3^4*(R3+T3))</f>
+        <v>1.1790643653749278</v>
       </c>
       <c r="AC3">
         <v>0</v>
@@ -1284,59 +1287,62 @@
         <v>5.39</v>
       </c>
       <c r="C4">
-        <v>0.2</v>
+        <f t="shared" ref="C4:C11" si="14">C3</f>
+        <v>0.14099999999999999</v>
       </c>
       <c r="D4">
         <v>5</v>
       </c>
       <c r="E4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0779999999999998</v>
       </c>
       <c r="F4">
-        <f t="shared" si="2"/>
-        <v>8.9442719099991588E-2</v>
+        <f t="shared" si="4"/>
+        <v>6.3057116965494056E-2</v>
       </c>
       <c r="G4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.8285577988678918</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H11" si="11">H3</f>
+        <f t="shared" ref="H4:H11" si="15">H3</f>
         <v>1</v>
       </c>
       <c r="I4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.849964616537755</v>
       </c>
       <c r="J4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0740552668330887</v>
       </c>
       <c r="K4">
-        <f>C4/SQRT(D4)</f>
-        <v>8.9442719099991588E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.3057116965494056E-2</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:M11" si="12">L3</f>
+        <f t="shared" ref="L4:M11" si="16">L3</f>
         <v>8.83</v>
       </c>
       <c r="M4">
-        <f t="shared" si="12"/>
-        <v>0.1</v>
+        <f t="shared" si="16"/>
+        <v>0.09</v>
       </c>
       <c r="N4">
         <f>N3</f>
         <v>16</v>
       </c>
       <c r="O4">
+        <f t="shared" ref="O4:O11" si="17">O3</f>
         <v>0.5</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4:P11" si="13">P3</f>
+        <f t="shared" ref="P4:Q11" si="18">P3</f>
         <v>16</v>
       </c>
       <c r="Q4">
+        <f t="shared" si="18"/>
         <v>0.1</v>
       </c>
       <c r="R4">
@@ -1344,36 +1350,36 @@
         <v>98000</v>
       </c>
       <c r="S4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.600000000000001</v>
       </c>
       <c r="T4">
-        <f t="shared" si="0"/>
-        <v>779.85922115028723</v>
+        <f t="shared" si="9"/>
+        <v>780.33668597956284</v>
       </c>
       <c r="U4">
-        <f t="shared" si="7"/>
-        <v>26.247940201611573</v>
+        <f t="shared" si="10"/>
+        <v>26.264010369081944</v>
       </c>
       <c r="V4">
-        <f t="shared" si="8"/>
-        <v>98779.859221150284</v>
+        <f t="shared" si="11"/>
+        <v>98780.336685979564</v>
       </c>
       <c r="W4">
-        <f t="shared" si="9"/>
-        <v>32.758424333709598</v>
+        <f t="shared" si="12"/>
+        <v>32.771302089896338</v>
       </c>
       <c r="X4">
-        <f>10^6*64*L4*N4/(E4^2*P4^4*(R4+T4))</f>
-        <v>1.2019179052610924</v>
+        <f t="shared" si="1"/>
+        <v>1.2019120956683464</v>
       </c>
       <c r="Y4">
-        <f>X4*SQRT((O4/N4)^2+(M4/L4)^2+4*(K4/E4)^2+16*(Q4/P4)^2+(W4/V4^2))</f>
-        <v>0.20561776217460312</v>
+        <f t="shared" si="2"/>
+        <v>0.14911413564624174</v>
       </c>
       <c r="Z4">
-        <f t="shared" si="10"/>
-        <v>1.2107627985709959</v>
+        <f t="shared" si="13"/>
+        <v>1.2107569462255565</v>
       </c>
       <c r="AB4" t="s">
         <v>27</v>
@@ -1390,59 +1396,62 @@
         <v>5.17</v>
       </c>
       <c r="C5">
-        <v>0.2</v>
+        <f t="shared" si="14"/>
+        <v>0.14099999999999999</v>
       </c>
       <c r="D5">
         <v>5</v>
       </c>
       <c r="E5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.034</v>
       </c>
       <c r="F5">
-        <f t="shared" si="2"/>
-        <v>8.9442719099991588E-2</v>
+        <f t="shared" si="4"/>
+        <v>6.3057116965494056E-2</v>
       </c>
       <c r="G5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.0765815349899288</v>
       </c>
       <c r="H5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="I5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.0971176100991</v>
       </c>
       <c r="J5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.030517321294949</v>
       </c>
       <c r="K5">
-        <f>C5/SQRT(D5)</f>
-        <v>8.9442719099991588E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.3057116965494056E-2</v>
       </c>
       <c r="L5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>8.83</v>
       </c>
       <c r="M5">
-        <f t="shared" si="12"/>
-        <v>0.1</v>
+        <f t="shared" si="16"/>
+        <v>0.09</v>
       </c>
       <c r="N5">
-        <f t="shared" ref="N5:N11" si="14">N4</f>
+        <f t="shared" ref="N5:N11" si="19">N4</f>
         <v>16</v>
       </c>
       <c r="O5">
+        <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
       <c r="P5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="Q5">
+        <f t="shared" si="18"/>
         <v>0.1</v>
       </c>
       <c r="R5">
@@ -1450,40 +1459,40 @@
         <v>98000</v>
       </c>
       <c r="S5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.600000000000001</v>
       </c>
       <c r="T5">
-        <f t="shared" si="0"/>
-        <v>779.85922115028723</v>
+        <f t="shared" si="9"/>
+        <v>780.33668597956284</v>
       </c>
       <c r="U5">
-        <f t="shared" si="7"/>
-        <v>26.247940201611573</v>
+        <f t="shared" si="10"/>
+        <v>26.264010369081944</v>
       </c>
       <c r="V5">
-        <f t="shared" si="8"/>
-        <v>98779.859221150284</v>
+        <f t="shared" si="11"/>
+        <v>98780.336685979564</v>
       </c>
       <c r="W5">
-        <f t="shared" si="9"/>
-        <v>32.758424333709598</v>
+        <f t="shared" si="12"/>
+        <v>32.771302089896338</v>
       </c>
       <c r="X5">
-        <f>10^6*64*L5*N5/(E5^2*P5^4*(R5+T5))</f>
-        <v>1.3063851926355281</v>
+        <f t="shared" si="1"/>
+        <v>1.3063788780894969</v>
       </c>
       <c r="Y5">
-        <f>X5*SQRT((O5/N5)^2+(M5/L5)^2+4*(K5/E5)^2+16*(Q5/P5)^2+(W5/V5^2))</f>
-        <v>0.23244837623493153</v>
+        <f t="shared" si="2"/>
+        <v>0.16822125966721291</v>
       </c>
       <c r="Z5">
-        <f t="shared" si="10"/>
-        <v>1.315230085945432</v>
+        <f t="shared" si="13"/>
+        <v>1.3152237286467072</v>
       </c>
       <c r="AB5">
         <f>AVERAGE(Y2:Y11)</f>
-        <v>0.22688377382080477</v>
+        <v>0.16373279207956717</v>
       </c>
       <c r="AC5">
         <v>0</v>
@@ -1497,59 +1506,62 @@
         <v>4.3600000000000003</v>
       </c>
       <c r="C6">
-        <v>0.2</v>
+        <f t="shared" si="14"/>
+        <v>0.14099999999999999</v>
       </c>
       <c r="D6">
         <v>4</v>
       </c>
       <c r="E6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0900000000000001</v>
       </c>
       <c r="F6">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
+        <f t="shared" si="4"/>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="G6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.7643901900730148</v>
       </c>
       <c r="H6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="I6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.7860344160236385</v>
       </c>
       <c r="J6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0859225603254545</v>
       </c>
       <c r="K6">
-        <f>C6/SQRT(D6)</f>
-        <v>0.1</v>
+        <f t="shared" si="0"/>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="L6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>8.83</v>
       </c>
       <c r="M6">
-        <f t="shared" si="12"/>
-        <v>0.1</v>
+        <f t="shared" si="16"/>
+        <v>0.09</v>
       </c>
       <c r="N6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>16</v>
       </c>
       <c r="O6">
+        <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
       <c r="P6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="Q6">
+        <f t="shared" si="18"/>
         <v>0.1</v>
       </c>
       <c r="R6">
@@ -1557,36 +1569,36 @@
         <v>98000</v>
       </c>
       <c r="S6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.600000000000001</v>
       </c>
       <c r="T6">
-        <f t="shared" si="0"/>
-        <v>779.85922115028723</v>
+        <f t="shared" si="9"/>
+        <v>780.33668597956284</v>
       </c>
       <c r="U6">
-        <f t="shared" si="7"/>
-        <v>26.247940201611573</v>
+        <f t="shared" si="10"/>
+        <v>26.264010369081944</v>
       </c>
       <c r="V6">
-        <f t="shared" si="8"/>
-        <v>98779.859221150284</v>
+        <f t="shared" si="11"/>
+        <v>98780.336685979564</v>
       </c>
       <c r="W6">
-        <f t="shared" si="9"/>
-        <v>32.758424333709598</v>
+        <f t="shared" si="12"/>
+        <v>32.771302089896338</v>
       </c>
       <c r="X6">
-        <f>10^6*64*L6*N6/(E6^2*P6^4*(R6+T6))</f>
-        <v>1.1755993325624363</v>
+        <f t="shared" si="1"/>
+        <v>1.1755936501831949</v>
       </c>
       <c r="Y6">
-        <f>X6*SQRT((O6/N6)^2+(M6/L6)^2+4*(K6/E6)^2+16*(Q6/P6)^2+(W6/V6^2))</f>
-        <v>0.22117839020442284</v>
+        <f t="shared" si="2"/>
+        <v>0.1596337287816863</v>
       </c>
       <c r="Z6">
-        <f t="shared" si="10"/>
-        <v>1.18444422587234</v>
+        <f t="shared" si="13"/>
+        <v>1.1844385007404052</v>
       </c>
       <c r="AC6">
         <v>0</v>
@@ -1600,59 +1612,62 @@
         <v>4.37</v>
       </c>
       <c r="C7">
-        <v>0.2</v>
+        <f t="shared" si="14"/>
+        <v>0.14099999999999999</v>
       </c>
       <c r="D7">
         <v>4</v>
       </c>
       <c r="E7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0925</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
+        <f t="shared" si="4"/>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="G7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.7511993658394385</v>
       </c>
       <c r="H7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="I7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.7728930481719445</v>
       </c>
       <c r="J7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0883945458108273</v>
       </c>
       <c r="K7">
-        <f>C7/SQRT(D7)</f>
-        <v>0.1</v>
+        <f t="shared" si="0"/>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="L7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>8.83</v>
       </c>
       <c r="M7">
-        <f t="shared" si="12"/>
-        <v>0.1</v>
+        <f t="shared" si="16"/>
+        <v>0.09</v>
       </c>
       <c r="N7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>16</v>
       </c>
       <c r="O7">
+        <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
       <c r="P7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="Q7">
+        <f t="shared" si="18"/>
         <v>0.1</v>
       </c>
       <c r="R7">
@@ -1660,36 +1675,36 @@
         <v>98000</v>
       </c>
       <c r="S7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.600000000000001</v>
       </c>
       <c r="T7">
-        <f t="shared" si="0"/>
-        <v>779.85922115028723</v>
+        <f t="shared" si="9"/>
+        <v>780.33668597956284</v>
       </c>
       <c r="U7">
-        <f t="shared" si="7"/>
-        <v>26.247940201611573</v>
+        <f t="shared" si="10"/>
+        <v>26.264010369081944</v>
       </c>
       <c r="V7">
-        <f t="shared" si="8"/>
-        <v>98779.859221150284</v>
+        <f t="shared" si="11"/>
+        <v>98780.336685979564</v>
       </c>
       <c r="W7">
-        <f t="shared" si="9"/>
-        <v>32.758424333709598</v>
+        <f t="shared" si="12"/>
+        <v>32.771302089896338</v>
       </c>
       <c r="X7">
-        <f>10^6*64*L7*N7/(E7^2*P7^4*(R7+T7))</f>
-        <v>1.1702251712204017</v>
+        <f t="shared" si="1"/>
+        <v>1.1702195148177172</v>
       </c>
       <c r="Y7">
-        <f>X7*SQRT((O7/N7)^2+(M7/L7)^2+4*(K7/E7)^2+16*(Q7/P7)^2+(W7/V7^2))</f>
-        <v>0.21968812288076248</v>
+        <f t="shared" si="2"/>
+        <v>0.15857401832191509</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="10"/>
-        <v>1.1790700645303058</v>
+        <f t="shared" si="13"/>
+        <v>1.1790643653749278</v>
       </c>
       <c r="AB7" t="s">
         <v>35</v>
@@ -1706,59 +1721,62 @@
         <v>4.43</v>
       </c>
       <c r="C8">
-        <v>0.2</v>
+        <f t="shared" si="14"/>
+        <v>0.14099999999999999</v>
       </c>
       <c r="D8">
         <v>4</v>
       </c>
       <c r="E8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.1074999999999999</v>
       </c>
       <c r="F8">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
+        <f t="shared" si="4"/>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="G8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.673305017769378</v>
       </c>
       <c r="H8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="I8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.6952954115346115</v>
       </c>
       <c r="J8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.1032237756191414</v>
       </c>
       <c r="K8">
-        <f>C8/SQRT(D8)</f>
-        <v>0.1</v>
+        <f t="shared" si="0"/>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="L8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>8.83</v>
       </c>
       <c r="M8">
-        <f t="shared" si="12"/>
-        <v>0.1</v>
+        <f t="shared" si="16"/>
+        <v>0.09</v>
       </c>
       <c r="N8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>16</v>
       </c>
       <c r="O8">
+        <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
       <c r="P8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="Q8">
+        <f t="shared" si="18"/>
         <v>0.1</v>
       </c>
       <c r="R8">
@@ -1766,40 +1784,40 @@
         <v>98000</v>
       </c>
       <c r="S8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.600000000000001</v>
       </c>
       <c r="T8">
-        <f t="shared" si="0"/>
-        <v>779.85922115028723</v>
+        <f t="shared" si="9"/>
+        <v>780.33668597956284</v>
       </c>
       <c r="U8">
-        <f t="shared" si="7"/>
-        <v>26.247940201611573</v>
+        <f t="shared" si="10"/>
+        <v>26.264010369081944</v>
       </c>
       <c r="V8">
-        <f t="shared" si="8"/>
-        <v>98779.859221150284</v>
+        <f t="shared" si="11"/>
+        <v>98780.336685979564</v>
       </c>
       <c r="W8">
-        <f t="shared" si="9"/>
-        <v>32.758424333709598</v>
+        <f t="shared" si="12"/>
+        <v>32.771302089896338</v>
       </c>
       <c r="X8">
-        <f>10^6*64*L8*N8/(E8^2*P8^4*(R8+T8))</f>
-        <v>1.1387407361198729</v>
+        <f t="shared" si="1"/>
+        <v>1.138735231900416</v>
       </c>
       <c r="Y8">
-        <f>X8*SQRT((O8/N8)^2+(M8/L8)^2+4*(K8/E8)^2+16*(Q8/P8)^2+(W8/V8^2))</f>
-        <v>0.21102513743854087</v>
+        <f t="shared" si="2"/>
+        <v>0.15241301904268706</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="10"/>
-        <v>1.1475856294297764</v>
+        <f t="shared" si="13"/>
+        <v>1.1475800824576257</v>
       </c>
       <c r="AB8">
         <f>AVERAGE(Z2:Z11)</f>
-        <v>1.2095078424646455</v>
+        <v>1.2095019961851645</v>
       </c>
       <c r="AC8">
         <v>0</v>
@@ -1813,59 +1831,62 @@
         <v>4.29</v>
       </c>
       <c r="C9">
-        <v>0.2</v>
+        <f t="shared" si="14"/>
+        <v>0.14099999999999999</v>
       </c>
       <c r="D9">
         <v>4</v>
       </c>
       <c r="E9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0725</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
+        <f t="shared" si="4"/>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="G9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.8584478388620846</v>
       </c>
       <c r="H9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="I9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.8797458346996452</v>
       </c>
       <c r="J9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0686151210991164</v>
       </c>
       <c r="K9">
-        <f>C9/SQRT(D9)</f>
-        <v>0.1</v>
+        <f t="shared" si="0"/>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="L9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>8.83</v>
       </c>
       <c r="M9">
-        <f t="shared" si="12"/>
-        <v>0.1</v>
+        <f t="shared" si="16"/>
+        <v>0.09</v>
       </c>
       <c r="N9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>16</v>
       </c>
       <c r="O9">
+        <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
       <c r="P9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="Q9">
+        <f t="shared" si="18"/>
         <v>0.1</v>
       </c>
       <c r="R9">
@@ -1873,36 +1894,36 @@
         <v>98000</v>
       </c>
       <c r="S9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.600000000000001</v>
       </c>
       <c r="T9">
-        <f t="shared" si="0"/>
-        <v>779.85922115028723</v>
+        <f t="shared" si="9"/>
+        <v>780.33668597956284</v>
       </c>
       <c r="U9">
-        <f t="shared" si="7"/>
-        <v>26.247940201611573</v>
+        <f t="shared" si="10"/>
+        <v>26.264010369081944</v>
       </c>
       <c r="V9">
-        <f t="shared" si="8"/>
-        <v>98779.859221150284</v>
+        <f t="shared" si="11"/>
+        <v>98780.336685979564</v>
       </c>
       <c r="W9">
-        <f t="shared" si="9"/>
-        <v>32.758424333709598</v>
+        <f t="shared" si="12"/>
+        <v>32.771302089896338</v>
       </c>
       <c r="X9">
-        <f>10^6*64*L9*N9/(E9^2*P9^4*(R9+T9))</f>
-        <v>1.2142768770153873</v>
+        <f t="shared" si="1"/>
+        <v>1.2142710076842915</v>
       </c>
       <c r="Y9">
-        <f>X9*SQRT((O9/N9)^2+(M9/L9)^2+4*(K9/E9)^2+16*(Q9/P9)^2+(W9/V9^2))</f>
-        <v>0.23200215033853183</v>
+        <f t="shared" si="2"/>
+        <v>0.16732913640305264</v>
       </c>
       <c r="Z9">
-        <f t="shared" si="10"/>
-        <v>1.2231217703252903</v>
+        <f t="shared" si="13"/>
+        <v>1.2231158582415007</v>
       </c>
       <c r="AC9">
         <v>0</v>
@@ -1916,59 +1937,62 @@
         <v>4.37</v>
       </c>
       <c r="C10">
-        <v>0.2</v>
+        <f t="shared" si="14"/>
+        <v>0.14099999999999999</v>
       </c>
       <c r="D10">
         <v>4</v>
       </c>
       <c r="E10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0925</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
+        <f t="shared" si="4"/>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="G10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.7511993658394385</v>
       </c>
       <c r="H10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="I10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.7728930481719445</v>
       </c>
       <c r="J10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0883945458108273</v>
       </c>
       <c r="K10">
-        <f>C10/SQRT(D10)</f>
-        <v>0.1</v>
+        <f t="shared" si="0"/>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="L10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>8.83</v>
       </c>
       <c r="M10">
-        <f t="shared" si="12"/>
-        <v>0.1</v>
+        <f t="shared" si="16"/>
+        <v>0.09</v>
       </c>
       <c r="N10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>16</v>
       </c>
       <c r="O10">
+        <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
       <c r="P10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="Q10">
+        <f t="shared" si="18"/>
         <v>0.1</v>
       </c>
       <c r="R10">
@@ -1976,36 +2000,36 @@
         <v>98000</v>
       </c>
       <c r="S10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.600000000000001</v>
       </c>
       <c r="T10">
-        <f t="shared" si="0"/>
-        <v>779.85922115028723</v>
+        <f t="shared" si="9"/>
+        <v>780.33668597956284</v>
       </c>
       <c r="U10">
-        <f t="shared" si="7"/>
-        <v>26.247940201611573</v>
+        <f t="shared" si="10"/>
+        <v>26.264010369081944</v>
       </c>
       <c r="V10">
-        <f t="shared" si="8"/>
-        <v>98779.859221150284</v>
+        <f t="shared" si="11"/>
+        <v>98780.336685979564</v>
       </c>
       <c r="W10">
-        <f t="shared" si="9"/>
-        <v>32.758424333709598</v>
+        <f t="shared" si="12"/>
+        <v>32.771302089896338</v>
       </c>
       <c r="X10">
-        <f>10^6*64*L10*N10/(E10^2*P10^4*(R10+T10))</f>
-        <v>1.1702251712204017</v>
+        <f t="shared" si="1"/>
+        <v>1.1702195148177172</v>
       </c>
       <c r="Y10">
-        <f>X10*SQRT((O10/N10)^2+(M10/L10)^2+4*(K10/E10)^2+16*(Q10/P10)^2+(W10/V10^2))</f>
-        <v>0.21968812288076248</v>
+        <f t="shared" si="2"/>
+        <v>0.15857401832191509</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="10"/>
-        <v>1.1790700645303058</v>
+        <f t="shared" si="13"/>
+        <v>1.1790643653749278</v>
       </c>
       <c r="AB10" t="s">
         <v>36</v>
@@ -2022,59 +2046,62 @@
         <v>4.26</v>
       </c>
       <c r="C11">
-        <v>0.2</v>
+        <f t="shared" si="14"/>
+        <v>0.14099999999999999</v>
       </c>
       <c r="D11">
         <v>4</v>
       </c>
       <c r="E11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0649999999999999</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
+        <f t="shared" si="4"/>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="G11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.8997045137836492</v>
       </c>
       <c r="H11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="I11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.9208541064578819</v>
       </c>
       <c r="J11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0611957657133468</v>
       </c>
       <c r="K11">
-        <f>C11/SQRT(D11)</f>
-        <v>0.1</v>
+        <f t="shared" si="0"/>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="L11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>8.83</v>
       </c>
       <c r="M11">
-        <f t="shared" si="12"/>
-        <v>0.1</v>
+        <f t="shared" si="16"/>
+        <v>0.09</v>
       </c>
       <c r="N11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>16</v>
       </c>
       <c r="O11">
+        <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
       <c r="P11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="Q11">
+        <f t="shared" si="18"/>
         <v>0.1</v>
       </c>
       <c r="R11">
@@ -2082,36 +2109,36 @@
         <v>98000</v>
       </c>
       <c r="S11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.600000000000001</v>
       </c>
       <c r="T11">
-        <f t="shared" si="0"/>
-        <v>779.85922115028723</v>
+        <f t="shared" si="9"/>
+        <v>780.33668597956284</v>
       </c>
       <c r="U11">
-        <f t="shared" si="7"/>
-        <v>26.247940201611573</v>
+        <f t="shared" si="10"/>
+        <v>26.264010369081944</v>
       </c>
       <c r="V11">
-        <f t="shared" si="8"/>
-        <v>98779.859221150284</v>
+        <f t="shared" si="11"/>
+        <v>98780.336685979564</v>
       </c>
       <c r="W11">
-        <f t="shared" si="9"/>
-        <v>32.758424333709598</v>
+        <f t="shared" si="12"/>
+        <v>32.771302089896338</v>
       </c>
       <c r="X11">
-        <f>10^6*64*L11*N11/(E11^2*P11^4*(R11+T11))</f>
-        <v>1.2314395882804832</v>
+        <f t="shared" si="1"/>
+        <v>1.2314336359916722</v>
       </c>
       <c r="Y11">
-        <f>X11*SQRT((O11/N11)^2+(M11/L11)^2+4*(K11/E11)^2+16*(Q11/P11)^2+(W11/V11^2))</f>
-        <v>0.23685994925915629</v>
+        <f t="shared" si="2"/>
+        <v>0.17078222804390636</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="10"/>
-        <v>1.2402844815903864</v>
+        <f t="shared" si="13"/>
+        <v>1.2402784865488821</v>
       </c>
       <c r="AC11">
         <v>0</v>

</xml_diff>

<commit_message>
Luftdruck in schwing korrigiert
</commit_message>
<xml_diff>
--- a/Versuch10/datasets/schwing1.xlsx
+++ b/Versuch10/datasets/schwing1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michele Calvanese\Uni\Grundpraktikum\Versuch10\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{825D1683-4873-4A84-914B-2F326E6F546A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A4DDACBC-99FC-486E-BEEB-D828B8E32E7A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17040" windowHeight="5916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -976,9 +976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1131,11 +1129,11 @@
         <v>0.1</v>
       </c>
       <c r="R2">
-        <v>98000</v>
+        <v>94888</v>
       </c>
       <c r="S2">
         <f>R2*0.0002</f>
-        <v>19.600000000000001</v>
+        <v>18.977600000000002</v>
       </c>
       <c r="T2">
         <f>4000*N2*9.806/(P2^2*PI())</f>
@@ -1147,27 +1145,27 @@
       </c>
       <c r="V2">
         <f>R2+T2</f>
-        <v>98780.336685979564</v>
+        <v>95668.336685979564</v>
       </c>
       <c r="W2">
         <f>SQRT(S2^2+U2^2)</f>
-        <v>32.771302089896338</v>
+        <v>32.402894044008541</v>
       </c>
       <c r="X2">
         <f t="shared" ref="X2:X11" si="1">10^6*64*L2*N2/(E2^2*P2^4*(R2+T2))</f>
-        <v>1.2275884123089735</v>
+        <v>1.2675206957733038</v>
       </c>
       <c r="Y2">
         <f t="shared" ref="Y2:Y11" si="2">X2*SQRT((O2/N2)^2+(M2/L2)^2+4*(K2/E2)^2+16*(Q2/P2)^2+(W2/V2^2))</f>
-        <v>0.19411235824513914</v>
+        <v>0.20042664936270468</v>
       </c>
       <c r="Z2">
         <f>10^6*64*L2*N2/(J2^2*P2^4*(R2+T2))</f>
-        <v>1.2364332628661832</v>
+        <v>1.276653260906595</v>
       </c>
       <c r="AB2">
         <f>AVERAGE(X2:X11)</f>
-        <v>1.2006571456279542</v>
+        <v>1.2397133806021094</v>
       </c>
       <c r="AC2">
         <v>0</v>
@@ -1216,64 +1214,64 @@
         <v>7.0499999999999993E-2</v>
       </c>
       <c r="L3">
-        <f>L2</f>
+        <f t="shared" ref="L3:R3" si="8">L2</f>
         <v>8.83</v>
       </c>
       <c r="M3">
-        <f>M2</f>
+        <f t="shared" si="8"/>
         <v>0.09</v>
       </c>
       <c r="N3">
-        <f>N2</f>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="O3">
-        <f>O2</f>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="P3">
-        <f>P2</f>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="Q3">
-        <f>Q2</f>
+        <f t="shared" si="8"/>
         <v>0.1</v>
       </c>
       <c r="R3">
-        <f>R2</f>
-        <v>98000</v>
+        <f t="shared" si="8"/>
+        <v>94888</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S11" si="8">R3*0.0002</f>
-        <v>19.600000000000001</v>
+        <f t="shared" ref="S3:S11" si="9">R3*0.0002</f>
+        <v>18.977600000000002</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T11" si="9">4000*N3*9.806/(P3^2*PI())</f>
+        <f t="shared" ref="T3:T11" si="10">4000*N3*9.806/(P3^2*PI())</f>
         <v>780.33668597956284</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U11" si="10">T3*SQRT((O3/N3)^2+4*(Q3/P3)^2)</f>
+        <f t="shared" ref="U3:U11" si="11">T3*SQRT((O3/N3)^2+4*(Q3/P3)^2)</f>
         <v>26.264010369081944</v>
       </c>
       <c r="V3">
-        <f t="shared" ref="V3:V11" si="11">R3+T3</f>
-        <v>98780.336685979564</v>
+        <f t="shared" ref="V3:V11" si="12">R3+T3</f>
+        <v>95668.336685979564</v>
       </c>
       <c r="W3">
-        <f t="shared" ref="W3:W11" si="12">SQRT(S3^2+U3^2)</f>
-        <v>32.771302089896338</v>
+        <f t="shared" ref="W3:W11" si="13">SQRT(S3^2+U3^2)</f>
+        <v>32.402894044008541</v>
       </c>
       <c r="X3">
         <f t="shared" si="1"/>
-        <v>1.1702195148177172</v>
+        <v>1.2082856426115587</v>
       </c>
       <c r="Y3">
         <f t="shared" si="2"/>
-        <v>0.15857401832191509</v>
+        <v>0.16373228112500673</v>
       </c>
       <c r="Z3">
-        <f t="shared" ref="Z3:Z11" si="13">10^6*64*L3*N3/(J3^2*P3^4*(R3+T3))</f>
-        <v>1.1790643653749278</v>
+        <f t="shared" ref="Z3:Z11" si="14">10^6*64*L3*N3/(J3^2*P3^4*(R3+T3))</f>
+        <v>1.2174182077448508</v>
       </c>
       <c r="AC3">
         <v>0</v>
@@ -1287,7 +1285,7 @@
         <v>5.39</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C11" si="14">C3</f>
+        <f t="shared" ref="C4:C11" si="15">C3</f>
         <v>0.14099999999999999</v>
       </c>
       <c r="D4">
@@ -1306,7 +1304,7 @@
         <v>5.8285577988678918</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H11" si="15">H3</f>
+        <f t="shared" ref="H4:H11" si="16">H3</f>
         <v>1</v>
       </c>
       <c r="I4">
@@ -1322,11 +1320,11 @@
         <v>6.3057116965494056E-2</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:M11" si="16">L3</f>
+        <f t="shared" ref="L4:M11" si="17">L3</f>
         <v>8.83</v>
       </c>
       <c r="M4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.09</v>
       </c>
       <c r="N4">
@@ -1334,52 +1332,52 @@
         <v>16</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O11" si="17">O3</f>
+        <f t="shared" ref="O4:O11" si="18">O3</f>
         <v>0.5</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4:Q11" si="18">P3</f>
+        <f t="shared" ref="P4:Q11" si="19">P3</f>
         <v>16</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.1</v>
       </c>
       <c r="R4">
         <f>R2</f>
-        <v>98000</v>
+        <v>94888</v>
       </c>
       <c r="S4">
-        <f t="shared" si="8"/>
-        <v>19.600000000000001</v>
+        <f t="shared" si="9"/>
+        <v>18.977600000000002</v>
       </c>
       <c r="T4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>780.33668597956284</v>
       </c>
       <c r="U4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>26.264010369081944</v>
       </c>
       <c r="V4">
-        <f t="shared" si="11"/>
-        <v>98780.336685979564</v>
+        <f t="shared" si="12"/>
+        <v>95668.336685979564</v>
       </c>
       <c r="W4">
-        <f t="shared" si="12"/>
-        <v>32.771302089896338</v>
+        <f t="shared" si="13"/>
+        <v>32.402894044008541</v>
       </c>
       <c r="X4">
         <f t="shared" si="1"/>
-        <v>1.2019120956683464</v>
+        <v>1.2410091529737031</v>
       </c>
       <c r="Y4">
         <f t="shared" si="2"/>
-        <v>0.14911413564624174</v>
+        <v>0.1539646775621514</v>
       </c>
       <c r="Z4">
-        <f t="shared" si="13"/>
-        <v>1.2107569462255565</v>
+        <f t="shared" si="14"/>
+        <v>1.2501417181069947</v>
       </c>
       <c r="AB4" t="s">
         <v>27</v>
@@ -1396,7 +1394,7 @@
         <v>5.17</v>
       </c>
       <c r="C5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.14099999999999999</v>
       </c>
       <c r="D5">
@@ -1415,7 +1413,7 @@
         <v>6.0765815349899288</v>
       </c>
       <c r="H5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="I5">
@@ -1431,68 +1429,68 @@
         <v>6.3057116965494056E-2</v>
       </c>
       <c r="L5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>8.83</v>
       </c>
       <c r="M5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.09</v>
       </c>
       <c r="N5">
-        <f t="shared" ref="N5:N11" si="19">N4</f>
+        <f t="shared" ref="N5:N11" si="20">N4</f>
         <v>16</v>
       </c>
       <c r="O5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.5</v>
       </c>
       <c r="P5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>16</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.1</v>
       </c>
       <c r="R5">
         <f>R2</f>
-        <v>98000</v>
+        <v>94888</v>
       </c>
       <c r="S5">
-        <f t="shared" si="8"/>
-        <v>19.600000000000001</v>
+        <f t="shared" si="9"/>
+        <v>18.977600000000002</v>
       </c>
       <c r="T5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>780.33668597956284</v>
       </c>
       <c r="U5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>26.264010369081944</v>
       </c>
       <c r="V5">
-        <f t="shared" si="11"/>
-        <v>98780.336685979564</v>
+        <f t="shared" si="12"/>
+        <v>95668.336685979564</v>
       </c>
       <c r="W5">
-        <f t="shared" si="12"/>
-        <v>32.771302089896338</v>
+        <f t="shared" si="13"/>
+        <v>32.402894044008541</v>
       </c>
       <c r="X5">
         <f t="shared" si="1"/>
-        <v>1.3063788780894969</v>
+        <v>1.348874140466211</v>
       </c>
       <c r="Y5">
         <f t="shared" si="2"/>
-        <v>0.16822125966721291</v>
+        <v>0.1736933381972125</v>
       </c>
       <c r="Z5">
-        <f t="shared" si="13"/>
-        <v>1.3152237286467072</v>
+        <f t="shared" si="14"/>
+        <v>1.3580067055995029</v>
       </c>
       <c r="AB5">
         <f>AVERAGE(Y2:Y11)</f>
-        <v>0.16373279207956717</v>
+        <v>0.1690588649051564</v>
       </c>
       <c r="AC5">
         <v>0</v>
@@ -1506,7 +1504,7 @@
         <v>4.3600000000000003</v>
       </c>
       <c r="C6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.14099999999999999</v>
       </c>
       <c r="D6">
@@ -1525,7 +1523,7 @@
         <v>5.7643901900730148</v>
       </c>
       <c r="H6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="I6">
@@ -1541,64 +1539,64 @@
         <v>7.0499999999999993E-2</v>
       </c>
       <c r="L6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>8.83</v>
       </c>
       <c r="M6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.09</v>
       </c>
       <c r="N6">
+        <f t="shared" si="20"/>
+        <v>16</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="18"/>
+        <v>0.5</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="19"/>
         <v>16</v>
       </c>
-      <c r="O6">
-        <f t="shared" si="17"/>
-        <v>0.5</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="18"/>
-        <v>16</v>
-      </c>
       <c r="Q6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.1</v>
       </c>
       <c r="R6">
         <f>R2</f>
-        <v>98000</v>
+        <v>94888</v>
       </c>
       <c r="S6">
-        <f t="shared" si="8"/>
-        <v>19.600000000000001</v>
+        <f t="shared" si="9"/>
+        <v>18.977600000000002</v>
       </c>
       <c r="T6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>780.33668597956284</v>
       </c>
       <c r="U6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>26.264010369081944</v>
       </c>
       <c r="V6">
-        <f t="shared" si="11"/>
-        <v>98780.336685979564</v>
+        <f t="shared" si="12"/>
+        <v>95668.336685979564</v>
       </c>
       <c r="W6">
-        <f t="shared" si="12"/>
-        <v>32.771302089896338</v>
+        <f t="shared" si="13"/>
+        <v>32.402894044008541</v>
       </c>
       <c r="X6">
         <f t="shared" si="1"/>
-        <v>1.1755936501831949</v>
+        <v>1.2138345934890094</v>
       </c>
       <c r="Y6">
         <f t="shared" si="2"/>
-        <v>0.1596337287816863</v>
+        <v>0.16482646296015044</v>
       </c>
       <c r="Z6">
-        <f t="shared" si="13"/>
-        <v>1.1844385007404052</v>
+        <f t="shared" si="14"/>
+        <v>1.2229671586223012</v>
       </c>
       <c r="AC6">
         <v>0</v>
@@ -1612,7 +1610,7 @@
         <v>4.37</v>
       </c>
       <c r="C7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.14099999999999999</v>
       </c>
       <c r="D7">
@@ -1631,7 +1629,7 @@
         <v>5.7511993658394385</v>
       </c>
       <c r="H7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="I7">
@@ -1647,64 +1645,64 @@
         <v>7.0499999999999993E-2</v>
       </c>
       <c r="L7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>8.83</v>
       </c>
       <c r="M7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.09</v>
       </c>
       <c r="N7">
+        <f t="shared" si="20"/>
+        <v>16</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="18"/>
+        <v>0.5</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="19"/>
         <v>16</v>
       </c>
-      <c r="O7">
-        <f t="shared" si="17"/>
-        <v>0.5</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="18"/>
-        <v>16</v>
-      </c>
       <c r="Q7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.1</v>
       </c>
       <c r="R7">
         <f>R2</f>
-        <v>98000</v>
+        <v>94888</v>
       </c>
       <c r="S7">
-        <f t="shared" si="8"/>
-        <v>19.600000000000001</v>
+        <f t="shared" si="9"/>
+        <v>18.977600000000002</v>
       </c>
       <c r="T7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>780.33668597956284</v>
       </c>
       <c r="U7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>26.264010369081944</v>
       </c>
       <c r="V7">
-        <f t="shared" si="11"/>
-        <v>98780.336685979564</v>
+        <f t="shared" si="12"/>
+        <v>95668.336685979564</v>
       </c>
       <c r="W7">
-        <f t="shared" si="12"/>
-        <v>32.771302089896338</v>
+        <f t="shared" si="13"/>
+        <v>32.402894044008541</v>
       </c>
       <c r="X7">
         <f t="shared" si="1"/>
-        <v>1.1702195148177172</v>
+        <v>1.2082856426115587</v>
       </c>
       <c r="Y7">
         <f t="shared" si="2"/>
-        <v>0.15857401832191509</v>
+        <v>0.16373228112500673</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="13"/>
-        <v>1.1790643653749278</v>
+        <f t="shared" si="14"/>
+        <v>1.2174182077448508</v>
       </c>
       <c r="AB7" t="s">
         <v>35</v>
@@ -1721,7 +1719,7 @@
         <v>4.43</v>
       </c>
       <c r="C8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.14099999999999999</v>
       </c>
       <c r="D8">
@@ -1740,7 +1738,7 @@
         <v>5.673305017769378</v>
       </c>
       <c r="H8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="I8">
@@ -1756,68 +1754,68 @@
         <v>7.0499999999999993E-2</v>
       </c>
       <c r="L8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>8.83</v>
       </c>
       <c r="M8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.09</v>
       </c>
       <c r="N8">
+        <f t="shared" si="20"/>
+        <v>16</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="18"/>
+        <v>0.5</v>
+      </c>
+      <c r="P8">
         <f t="shared" si="19"/>
         <v>16</v>
       </c>
-      <c r="O8">
-        <f t="shared" si="17"/>
-        <v>0.5</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="18"/>
-        <v>16</v>
-      </c>
       <c r="Q8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.1</v>
       </c>
       <c r="R8">
         <f>R2</f>
-        <v>98000</v>
+        <v>94888</v>
       </c>
       <c r="S8">
-        <f t="shared" si="8"/>
-        <v>19.600000000000001</v>
+        <f t="shared" si="9"/>
+        <v>18.977600000000002</v>
       </c>
       <c r="T8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>780.33668597956284</v>
       </c>
       <c r="U8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>26.264010369081944</v>
       </c>
       <c r="V8">
-        <f t="shared" si="11"/>
-        <v>98780.336685979564</v>
+        <f t="shared" si="12"/>
+        <v>95668.336685979564</v>
       </c>
       <c r="W8">
-        <f t="shared" si="12"/>
-        <v>32.771302089896338</v>
+        <f t="shared" si="13"/>
+        <v>32.402894044008541</v>
       </c>
       <c r="X8">
         <f t="shared" si="1"/>
-        <v>1.138735231900416</v>
+        <v>1.175777205916396</v>
       </c>
       <c r="Y8">
         <f t="shared" si="2"/>
-        <v>0.15241301904268706</v>
+        <v>0.15737087038709344</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="13"/>
-        <v>1.1475800824576257</v>
+        <f t="shared" si="14"/>
+        <v>1.1849097710496874</v>
       </c>
       <c r="AB8">
         <f>AVERAGE(Z2:Z11)</f>
-        <v>1.2095019961851645</v>
+        <v>1.2488459457354009</v>
       </c>
       <c r="AC8">
         <v>0</v>
@@ -1831,7 +1829,7 @@
         <v>4.29</v>
       </c>
       <c r="C9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.14099999999999999</v>
       </c>
       <c r="D9">
@@ -1850,7 +1848,7 @@
         <v>5.8584478388620846</v>
       </c>
       <c r="H9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="I9">
@@ -1866,64 +1864,64 @@
         <v>7.0499999999999993E-2</v>
       </c>
       <c r="L9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>8.83</v>
       </c>
       <c r="M9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.09</v>
       </c>
       <c r="N9">
+        <f t="shared" si="20"/>
+        <v>16</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="18"/>
+        <v>0.5</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="19"/>
         <v>16</v>
       </c>
-      <c r="O9">
-        <f t="shared" si="17"/>
-        <v>0.5</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="18"/>
-        <v>16</v>
-      </c>
       <c r="Q9">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.1</v>
       </c>
       <c r="R9">
         <f>R2</f>
-        <v>98000</v>
+        <v>94888</v>
       </c>
       <c r="S9">
-        <f t="shared" si="8"/>
-        <v>19.600000000000001</v>
+        <f t="shared" si="9"/>
+        <v>18.977600000000002</v>
       </c>
       <c r="T9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>780.33668597956284</v>
       </c>
       <c r="U9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>26.264010369081944</v>
       </c>
       <c r="V9">
-        <f t="shared" si="11"/>
-        <v>98780.336685979564</v>
+        <f t="shared" si="12"/>
+        <v>95668.336685979564</v>
       </c>
       <c r="W9">
-        <f t="shared" si="12"/>
-        <v>32.771302089896338</v>
+        <f t="shared" si="13"/>
+        <v>32.402894044008541</v>
       </c>
       <c r="X9">
         <f t="shared" si="1"/>
-        <v>1.2142710076842915</v>
+        <v>1.2537700886426761</v>
       </c>
       <c r="Y9">
         <f t="shared" si="2"/>
-        <v>0.16732913640305264</v>
+        <v>0.17277219488663539</v>
       </c>
       <c r="Z9">
-        <f t="shared" si="13"/>
-        <v>1.2231158582415007</v>
+        <f t="shared" si="14"/>
+        <v>1.2629026537759671</v>
       </c>
       <c r="AC9">
         <v>0</v>
@@ -1937,7 +1935,7 @@
         <v>4.37</v>
       </c>
       <c r="C10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.14099999999999999</v>
       </c>
       <c r="D10">
@@ -1956,7 +1954,7 @@
         <v>5.7511993658394385</v>
       </c>
       <c r="H10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="I10">
@@ -1972,64 +1970,64 @@
         <v>7.0499999999999993E-2</v>
       </c>
       <c r="L10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>8.83</v>
       </c>
       <c r="M10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.09</v>
       </c>
       <c r="N10">
+        <f t="shared" si="20"/>
+        <v>16</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="18"/>
+        <v>0.5</v>
+      </c>
+      <c r="P10">
         <f t="shared" si="19"/>
         <v>16</v>
       </c>
-      <c r="O10">
-        <f t="shared" si="17"/>
-        <v>0.5</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="18"/>
-        <v>16</v>
-      </c>
       <c r="Q10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.1</v>
       </c>
       <c r="R10">
         <f>R2</f>
-        <v>98000</v>
+        <v>94888</v>
       </c>
       <c r="S10">
-        <f t="shared" si="8"/>
-        <v>19.600000000000001</v>
+        <f t="shared" si="9"/>
+        <v>18.977600000000002</v>
       </c>
       <c r="T10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>780.33668597956284</v>
       </c>
       <c r="U10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>26.264010369081944</v>
       </c>
       <c r="V10">
-        <f t="shared" si="11"/>
-        <v>98780.336685979564</v>
+        <f t="shared" si="12"/>
+        <v>95668.336685979564</v>
       </c>
       <c r="W10">
-        <f t="shared" si="12"/>
-        <v>32.771302089896338</v>
+        <f t="shared" si="13"/>
+        <v>32.402894044008541</v>
       </c>
       <c r="X10">
         <f t="shared" si="1"/>
-        <v>1.1702195148177172</v>
+        <v>1.2082856426115587</v>
       </c>
       <c r="Y10">
         <f t="shared" si="2"/>
-        <v>0.15857401832191509</v>
+        <v>0.16373228112500673</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="13"/>
-        <v>1.1790643653749278</v>
+        <f t="shared" si="14"/>
+        <v>1.2174182077448508</v>
       </c>
       <c r="AB10" t="s">
         <v>36</v>
@@ -2046,7 +2044,7 @@
         <v>4.26</v>
       </c>
       <c r="C11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.14099999999999999</v>
       </c>
       <c r="D11">
@@ -2065,7 +2063,7 @@
         <v>5.8997045137836492</v>
       </c>
       <c r="H11">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="I11">
@@ -2081,64 +2079,64 @@
         <v>7.0499999999999993E-2</v>
       </c>
       <c r="L11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>8.83</v>
       </c>
       <c r="M11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.09</v>
       </c>
       <c r="N11">
+        <f t="shared" si="20"/>
+        <v>16</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="18"/>
+        <v>0.5</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="19"/>
         <v>16</v>
       </c>
-      <c r="O11">
-        <f t="shared" si="17"/>
-        <v>0.5</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="18"/>
-        <v>16</v>
-      </c>
       <c r="Q11">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.1</v>
       </c>
       <c r="R11">
         <f>R2</f>
-        <v>98000</v>
+        <v>94888</v>
       </c>
       <c r="S11">
-        <f t="shared" si="8"/>
-        <v>19.600000000000001</v>
+        <f t="shared" si="9"/>
+        <v>18.977600000000002</v>
       </c>
       <c r="T11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>780.33668597956284</v>
       </c>
       <c r="U11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>26.264010369081944</v>
       </c>
       <c r="V11">
-        <f t="shared" si="11"/>
-        <v>98780.336685979564</v>
+        <f t="shared" si="12"/>
+        <v>95668.336685979564</v>
       </c>
       <c r="W11">
-        <f t="shared" si="12"/>
-        <v>32.771302089896338</v>
+        <f t="shared" si="13"/>
+        <v>32.402894044008541</v>
       </c>
       <c r="X11">
         <f t="shared" si="1"/>
-        <v>1.2314336359916722</v>
+        <v>1.2714910009251184</v>
       </c>
       <c r="Y11">
         <f t="shared" si="2"/>
-        <v>0.17078222804390636</v>
+        <v>0.17633761232059583</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="13"/>
-        <v>1.2402784865488821</v>
+        <f t="shared" si="14"/>
+        <v>1.2806235660584098</v>
       </c>
       <c r="AC11">
         <v>0</v>

</xml_diff>